<commit_message>
change hardcoded coin units to configurable
</commit_message>
<xml_diff>
--- a/user_import_example.xlsx
+++ b/user_import_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cralix/PycharmProjects/protonCoin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2B34E5-238F-5B44-84BD-4D1C63A6DE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DBA10A-5676-9D46-92D1-5A37E897EFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="820" windowWidth="28240" windowHeight="17440" xr2:uid="{9CB81EE0-A314-E74A-A6A7-F03D691FA59C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Фамилия</t>
   </si>
@@ -46,19 +46,22 @@
     <t>Отчество (не обязательное поле)</t>
   </si>
   <si>
-    <t>Иванов</t>
-  </si>
-  <si>
-    <t>Иван</t>
-  </si>
-  <si>
-    <t>Иванович</t>
-  </si>
-  <si>
-    <t>Тестов</t>
-  </si>
-  <si>
-    <t>Тест</t>
+    <t>Федоров</t>
+  </si>
+  <si>
+    <t>Кирилл</t>
+  </si>
+  <si>
+    <t>Евгеньевич</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,6 +455,9 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>